<commit_message>
work on data processor
</commit_message>
<xml_diff>
--- a/tests/AppBundle/Resources/sample_data/people/pid1.xlsx
+++ b/tests/AppBundle/Resources/sample_data/people/pid1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,10 +28,10 @@
     <t xml:space="preserve">ExampleData</t>
   </si>
   <si>
-    <t xml:space="preserve">PID1_A</t>
+    <t xml:space="preserve">PID1_B</t>
   </si>
   <si>
-    <t xml:space="preserve">PID1_B</t>
+    <t xml:space="preserve">PID1_A</t>
   </si>
 </sst>
 </file>
@@ -131,13 +131,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -149,7 +146,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>12.321</v>
+        <v>14.392</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>2</v>
@@ -157,7 +154,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>14.392</v>
+        <v>12.321</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>3</v>

</xml_diff>